<commit_message>
"Changes in ExtentReportNg File"
</commit_message>
<xml_diff>
--- a/appium/Results/ExcelSheetsFolder/18062025/ExcelResults.xlsx
+++ b/appium/Results/ExcelSheetsFolder/18062025/ExcelResults.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="28">
   <si>
     <t>DeviceName</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>1280 720</t>
+  </si>
+  <si>
+    <t>src_fmt = invalid</t>
+  </si>
+  <si>
+    <t>NA NA</t>
   </si>
 </sst>
 </file>
@@ -608,7 +614,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -618,7 +624,7 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="18.17578125"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="28.09765625"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="11.375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.11328125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.1875"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="14.10546875"/>
   </cols>
   <sheetData>
@@ -1482,6 +1488,86 @@
         <v>11</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E44" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F44" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E45" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F45" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E46" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F46" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="F47" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>